<commit_message>
try changing the title of the country column
</commit_message>
<xml_diff>
--- a/data/country_performance_sel.xlsx
+++ b/data/country_performance_sel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Eastern Europe" sheetId="2" r:id="rId1"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
-  <si>
-    <t>NAME_ENGL</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>performance</t>
   </si>
@@ -80,6 +77,12 @@
   </si>
   <si>
     <t>El Salvador</t>
+  </si>
+  <si>
+    <t>Central America</t>
+  </si>
+  <si>
+    <t>Eastern Europe</t>
   </si>
 </sst>
 </file>
@@ -449,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,15 +464,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>-55</v>
@@ -477,7 +480,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -485,7 +488,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>-52</v>
@@ -493,7 +496,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>-9</v>
@@ -501,7 +504,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>-31</v>
@@ -509,7 +512,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>-35</v>
@@ -517,7 +520,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>11</v>
@@ -525,7 +528,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>-41</v>
@@ -533,7 +536,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>-4</v>
@@ -541,7 +544,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>-25</v>
@@ -556,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,15 +571,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -584,7 +587,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -592,7 +595,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>-8</v>
@@ -600,7 +603,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>-4</v>
@@ -608,7 +611,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>-1</v>
@@ -616,7 +619,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -624,7 +627,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -632,7 +635,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>0</v>

</xml_diff>